<commit_message>
fixing dollar sign add bug
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2300$$$$</t>
+          <t>2300$</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1000000$$$</t>
+          <t>1000000$</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5000$$</t>
+          <t>3000$</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -540,6 +540,28 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>checkemail@abv.bg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TestingDollar</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>b'$2b$12$hPMP1PTGHNPEXPrmm112puz6ZbREw6wV9/cAfbDVr7rcS54VyerBi'</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2750$</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>letstestthedollar@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>